<commit_message>
Added New 2 TC`s  (Edit/Delete Created Schema)
</commit_message>
<xml_diff>
--- a/src/test/resources/TestDataFiles/scheduleSchema/TestData.xlsx
+++ b/src/test/resources/TestDataFiles/scheduleSchema/TestData.xlsx
@@ -3,25 +3,21 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20228"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AFarid\git\qa\src\test\resources\TestDataFiles\scheduleSchema\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{106A63F9-FF95-47DF-8720-1898E288DD8D}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100800_{FCA6A0CF-6443-4B7F-B5A6-96CF91FE29A4}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="27660" windowHeight="10755" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18270" windowHeight="2295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TestData" sheetId="1" r:id="rId1"/>
     <sheet name="Lists" sheetId="2" state="hidden" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="76">
   <si>
     <t>Supported Browser Types</t>
   </si>
@@ -246,6 +242,9 @@
   </si>
   <si>
     <t>Schema-List View</t>
+  </si>
+  <si>
+    <t>Schema Delete</t>
   </si>
 </sst>
 </file>
@@ -702,8 +701,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:XFD967"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="C45" sqref="C45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -34157,6 +34156,9 @@
       <c r="B45" s="14" t="s">
         <v>72</v>
       </c>
+      <c r="C45" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="46" spans="1:16384" ht="15.75" customHeight="1">
       <c r="A46" s="13" t="s">

</xml_diff>